<commit_message>
Updated the script to accept single sheet and added correct filtering for missing values like "Yahrtzeit". Previously, set operation was saying all of the values were missing even if only in one case it was.
</commit_message>
<xml_diff>
--- a/uploads/output.xlsx
+++ b/uploads/output.xlsx
@@ -588,7 +588,11 @@
           <t>September 2 - Line 4 (35)</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Happy Birthday</t>
+        </is>
+      </c>
       <c r="E8" t="n">
         <v>35</v>
       </c>
@@ -607,7 +611,11 @@
           <t>September 2 - Line 3 (35)</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Ella Kalif</t>
+        </is>
+      </c>
       <c r="E9" t="n">
         <v>35</v>
       </c>
@@ -1215,11 +1223,7 @@
           <t>September 7 - Line 1 (25)</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>Yahrtzeit of Libby Echenberg</t>
-        </is>
-      </c>
+      <c r="D41" t="inlineStr"/>
       <c r="E41" t="n">
         <v>25</v>
       </c>
@@ -1618,11 +1622,7 @@
           <t>September 11 - Line 2 (35)</t>
         </is>
       </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>Yahrtzeit of Felicia Aaron</t>
-        </is>
-      </c>
+      <c r="D62" t="inlineStr"/>
       <c r="E62" t="n">
         <v>35</v>
       </c>
@@ -1641,11 +1641,7 @@
           <t>September 11 - Line 1 (35)</t>
         </is>
       </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>Tzipora Bas Shimon Leib</t>
-        </is>
-      </c>
+      <c r="D63" t="inlineStr"/>
       <c r="E63" t="n">
         <v>35</v>
       </c>
@@ -1664,7 +1660,11 @@
           <t>September 12 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D64" t="inlineStr"/>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E64" t="n">
         <v>35</v>
       </c>
@@ -1683,7 +1683,11 @@
           <t>September 12 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D65" t="inlineStr"/>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Larry Barnett</t>
+        </is>
+      </c>
       <c r="E65" t="n">
         <v>35</v>
       </c>
@@ -2310,7 +2314,11 @@
           <t>September 19 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D98" t="inlineStr"/>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E98" t="n">
         <v>35</v>
       </c>
@@ -2329,7 +2337,11 @@
           <t>September 19 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D99" t="inlineStr"/>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>Dave Lebowitz</t>
+        </is>
+      </c>
       <c r="E99" t="n">
         <v>35</v>
       </c>
@@ -2842,7 +2854,11 @@
           <t>September 24 - Line 3 (35)</t>
         </is>
       </c>
-      <c r="D126" t="inlineStr"/>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>Helen Sapolnick</t>
+        </is>
+      </c>
       <c r="E126" t="n">
         <v>35</v>
       </c>
@@ -2918,7 +2934,11 @@
           <t>September 25 - Line 3 (30)</t>
         </is>
       </c>
-      <c r="D130" t="inlineStr"/>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E130" t="n">
         <v>30</v>
       </c>
@@ -2937,7 +2957,11 @@
           <t>September 25 - Line 2 (30)</t>
         </is>
       </c>
-      <c r="D131" t="inlineStr"/>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>Susan Holland</t>
+        </is>
+      </c>
       <c r="E131" t="n">
         <v>30</v>
       </c>
@@ -3070,11 +3094,7 @@
           <t>September 26 - Line 1 (35)</t>
         </is>
       </c>
-      <c r="D138" t="inlineStr">
-        <is>
-          <t>Happy Birthday David Vineberg</t>
-        </is>
-      </c>
+      <c r="D138" t="inlineStr"/>
       <c r="E138" t="n">
         <v>35</v>
       </c>
@@ -3321,7 +3341,11 @@
           <t>September 29 - Line 4 (35)</t>
         </is>
       </c>
-      <c r="D151" t="inlineStr"/>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>Harry Wishnev</t>
+        </is>
+      </c>
       <c r="E151" t="n">
         <v>35</v>
       </c>
@@ -3454,7 +3478,11 @@
           <t>October 1 - Line 4 (35)</t>
         </is>
       </c>
-      <c r="D158" t="inlineStr"/>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>Happy Birthday</t>
+        </is>
+      </c>
       <c r="E158" t="n">
         <v>35</v>
       </c>
@@ -3473,7 +3501,11 @@
           <t>October 1 - Line 3 (35)</t>
         </is>
       </c>
-      <c r="D159" t="inlineStr"/>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>Danny Budanitsky</t>
+        </is>
+      </c>
       <c r="E159" t="n">
         <v>35</v>
       </c>
@@ -3720,7 +3752,11 @@
           <t>October 4 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D172" t="inlineStr"/>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>Happy Birthday</t>
+        </is>
+      </c>
       <c r="E172" t="n">
         <v>35</v>
       </c>
@@ -3739,7 +3775,11 @@
           <t>October 4 - Line 4 (35)</t>
         </is>
       </c>
-      <c r="D173" t="inlineStr"/>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>Eli Budanitsky</t>
+        </is>
+      </c>
       <c r="E173" t="n">
         <v>35</v>
       </c>
@@ -3758,7 +3798,11 @@
           <t>October 4 - Line 3 (35)</t>
         </is>
       </c>
-      <c r="D174" t="inlineStr"/>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E174" t="n">
         <v>35</v>
       </c>
@@ -3777,7 +3821,11 @@
           <t>October 4 - Line 2 (35)</t>
         </is>
       </c>
-      <c r="D175" t="inlineStr"/>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>Gilah Fernande Bohbot</t>
+        </is>
+      </c>
       <c r="E175" t="n">
         <v>35</v>
       </c>
@@ -3986,7 +4034,11 @@
           <t>October 7 - Line 4 (35)</t>
         </is>
       </c>
-      <c r="D186" t="inlineStr"/>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>Happy Birthday</t>
+        </is>
+      </c>
       <c r="E186" t="n">
         <v>35</v>
       </c>
@@ -4005,7 +4057,11 @@
           <t>October 7 - Line 3 (35)</t>
         </is>
       </c>
-      <c r="D187" t="inlineStr"/>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>Sheryl Smolensky</t>
+        </is>
+      </c>
       <c r="E187" t="n">
         <v>35</v>
       </c>
@@ -4062,7 +4118,11 @@
           <t>October 8 - Line 5 (25)</t>
         </is>
       </c>
-      <c r="D190" t="inlineStr"/>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E190" t="n">
         <v>25</v>
       </c>
@@ -4081,7 +4141,11 @@
           <t>October 8 - Line 4 (25)</t>
         </is>
       </c>
-      <c r="D191" t="inlineStr"/>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>Jeanette Holland</t>
+        </is>
+      </c>
       <c r="E191" t="n">
         <v>25</v>
       </c>
@@ -4385,7 +4449,11 @@
           <t>October 11 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D207" t="inlineStr"/>
+      <c r="D207" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E207" t="n">
         <v>35</v>
       </c>
@@ -4404,7 +4472,11 @@
           <t>October 11 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D208" t="inlineStr"/>
+      <c r="D208" t="inlineStr">
+        <is>
+          <t>Alvin Holland</t>
+        </is>
+      </c>
       <c r="E208" t="n">
         <v>35</v>
       </c>
@@ -4423,7 +4495,11 @@
           <t>October 11 - Line 4 (35)</t>
         </is>
       </c>
-      <c r="D209" t="inlineStr"/>
+      <c r="D209" t="inlineStr">
+        <is>
+          <t>Happy Anniversary</t>
+        </is>
+      </c>
       <c r="E209" t="n">
         <v>35</v>
       </c>
@@ -4442,7 +4518,11 @@
           <t>October 11 - Line 3 (35)</t>
         </is>
       </c>
-      <c r="D210" t="inlineStr"/>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>Kari &amp; Paul Saltin</t>
+        </is>
+      </c>
       <c r="E210" t="n">
         <v>35</v>
       </c>
@@ -4461,7 +4541,11 @@
           <t>October 11 - Line 2 (35)</t>
         </is>
       </c>
-      <c r="D211" t="inlineStr"/>
+      <c r="D211" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Yahrtzeit </t>
+        </is>
+      </c>
       <c r="E211" t="n">
         <v>35</v>
       </c>
@@ -4480,7 +4564,11 @@
           <t>October 11 - Line 1 (35)</t>
         </is>
       </c>
-      <c r="D212" t="inlineStr"/>
+      <c r="D212" t="inlineStr">
+        <is>
+          <t>Richard Hawkins</t>
+        </is>
+      </c>
       <c r="E212" t="n">
         <v>35</v>
       </c>
@@ -4537,7 +4625,11 @@
           <t>October 12 - Line 4 (35)</t>
         </is>
       </c>
-      <c r="D215" t="inlineStr"/>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E215" t="n">
         <v>35</v>
       </c>
@@ -4556,7 +4648,11 @@
           <t>October 12 - Line 3 (35)</t>
         </is>
       </c>
-      <c r="D216" t="inlineStr"/>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>Norman Mayberg</t>
+        </is>
+      </c>
       <c r="E216" t="n">
         <v>35</v>
       </c>
@@ -4575,7 +4671,11 @@
           <t>October 12 - Line 2 (35)</t>
         </is>
       </c>
-      <c r="D217" t="inlineStr"/>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>Happy Birthday</t>
+        </is>
+      </c>
       <c r="E217" t="n">
         <v>35</v>
       </c>
@@ -4594,7 +4694,11 @@
           <t>October 12 - Line 1 (35)</t>
         </is>
       </c>
-      <c r="D218" t="inlineStr"/>
+      <c r="D218" t="inlineStr">
+        <is>
+          <t>David Abayev</t>
+        </is>
+      </c>
       <c r="E218" t="n">
         <v>35</v>
       </c>
@@ -4670,7 +4774,11 @@
           <t>October 13 - Line 3 (35)</t>
         </is>
       </c>
-      <c r="D222" t="inlineStr"/>
+      <c r="D222" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E222" t="n">
         <v>35</v>
       </c>
@@ -4689,7 +4797,11 @@
           <t>October 13 - Line 2 (35)</t>
         </is>
       </c>
-      <c r="D223" t="inlineStr"/>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>Charles Chalom Benaroch</t>
+        </is>
+      </c>
       <c r="E223" t="n">
         <v>35</v>
       </c>
@@ -5126,7 +5238,11 @@
           <t>October 18 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D246" t="inlineStr"/>
+      <c r="D246" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E246" t="n">
         <v>35</v>
       </c>
@@ -5145,7 +5261,11 @@
           <t>October 18 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D247" t="inlineStr"/>
+      <c r="D247" t="inlineStr">
+        <is>
+          <t>Beverly Cogan</t>
+        </is>
+      </c>
       <c r="E247" t="n">
         <v>35</v>
       </c>
@@ -5506,7 +5626,11 @@
           <t>October 21 - Line 3 (35)</t>
         </is>
       </c>
-      <c r="D266" t="inlineStr"/>
+      <c r="D266" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E266" t="n">
         <v>35</v>
       </c>
@@ -5525,7 +5649,11 @@
           <t>October 21 - Line 2 (35)</t>
         </is>
       </c>
-      <c r="D267" t="inlineStr"/>
+      <c r="D267" t="inlineStr">
+        <is>
+          <t>Steven Hawkins</t>
+        </is>
+      </c>
       <c r="E267" t="n">
         <v>35</v>
       </c>
@@ -5791,7 +5919,11 @@
           <t>October 24 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D281" t="inlineStr"/>
+      <c r="D281" t="inlineStr">
+        <is>
+          <t>Happy Birthday</t>
+        </is>
+      </c>
       <c r="E281" t="n">
         <v>35</v>
       </c>
@@ -5810,7 +5942,11 @@
           <t>October 24 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D282" t="inlineStr"/>
+      <c r="D282" t="inlineStr">
+        <is>
+          <t>Jared Budanitsky</t>
+        </is>
+      </c>
       <c r="E282" t="n">
         <v>35</v>
       </c>
@@ -5829,7 +5965,11 @@
           <t>October 24 - Line 4 (35)</t>
         </is>
       </c>
-      <c r="D283" t="inlineStr"/>
+      <c r="D283" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E283" t="n">
         <v>35</v>
       </c>
@@ -5848,7 +5988,11 @@
           <t>October 24 - Line 3 (35)</t>
         </is>
       </c>
-      <c r="D284" t="inlineStr"/>
+      <c r="D284" t="inlineStr">
+        <is>
+          <t>Irene Lebowitz</t>
+        </is>
+      </c>
       <c r="E284" t="n">
         <v>35</v>
       </c>
@@ -6323,7 +6467,11 @@
           <t>October 29 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D309" t="inlineStr"/>
+      <c r="D309" t="inlineStr">
+        <is>
+          <t>Happy Birthday</t>
+        </is>
+      </c>
       <c r="E309" t="n">
         <v>35</v>
       </c>
@@ -6342,7 +6490,11 @@
           <t>October 29 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D310" t="inlineStr"/>
+      <c r="D310" t="inlineStr">
+        <is>
+          <t>Aaron Mitchell Rudnick</t>
+        </is>
+      </c>
       <c r="E310" t="n">
         <v>35</v>
       </c>
@@ -6437,7 +6589,11 @@
           <t>October 30 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D315" t="inlineStr"/>
+      <c r="D315" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E315" t="n">
         <v>35</v>
       </c>
@@ -6456,7 +6612,11 @@
           <t>October 30 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D316" t="inlineStr"/>
+      <c r="D316" t="inlineStr">
+        <is>
+          <t>Rachel Burke</t>
+        </is>
+      </c>
       <c r="E316" t="n">
         <v>35</v>
       </c>
@@ -6475,7 +6635,11 @@
           <t>October 30 - Line 4 (35)</t>
         </is>
       </c>
-      <c r="D317" t="inlineStr"/>
+      <c r="D317" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E317" t="n">
         <v>35</v>
       </c>
@@ -6494,7 +6658,11 @@
           <t>October 30 - Line 3 (35)</t>
         </is>
       </c>
-      <c r="D318" t="inlineStr"/>
+      <c r="D318" t="inlineStr">
+        <is>
+          <t>Andrew Kurs</t>
+        </is>
+      </c>
       <c r="E318" t="n">
         <v>35</v>
       </c>
@@ -7007,7 +7175,11 @@
           <t>November 4 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D345" t="inlineStr"/>
+      <c r="D345" t="inlineStr">
+        <is>
+          <t>Sholom Leverton</t>
+        </is>
+      </c>
       <c r="E345" t="n">
         <v>35</v>
       </c>
@@ -7026,7 +7198,11 @@
           <t>November 4 - Line 4 (35)</t>
         </is>
       </c>
-      <c r="D346" t="inlineStr"/>
+      <c r="D346" t="inlineStr">
+        <is>
+          <t>Happy Birthday</t>
+        </is>
+      </c>
       <c r="E346" t="n">
         <v>35</v>
       </c>
@@ -7045,7 +7221,11 @@
           <t>November 4 - Line 3 (35)</t>
         </is>
       </c>
-      <c r="D347" t="inlineStr"/>
+      <c r="D347" t="inlineStr">
+        <is>
+          <t>Sholom Kaye</t>
+        </is>
+      </c>
       <c r="E347" t="n">
         <v>35</v>
       </c>
@@ -7102,7 +7282,11 @@
           <t>November 5 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D350" t="inlineStr"/>
+      <c r="D350" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E350" t="n">
         <v>35</v>
       </c>
@@ -7121,7 +7305,11 @@
           <t>November 5 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D351" t="inlineStr"/>
+      <c r="D351" t="inlineStr">
+        <is>
+          <t>Phoebe Herman</t>
+        </is>
+      </c>
       <c r="E351" t="n">
         <v>35</v>
       </c>
@@ -7197,11 +7385,7 @@
           <t>November 5 - Line 1 (35)</t>
         </is>
       </c>
-      <c r="D355" t="inlineStr">
-        <is>
-          <t>Happy Birthday Shulamit Perlo</t>
-        </is>
-      </c>
+      <c r="D355" t="inlineStr"/>
       <c r="E355" t="n">
         <v>35</v>
       </c>
@@ -7600,7 +7784,11 @@
           <t>November 9 - Line 4 (35)</t>
         </is>
       </c>
-      <c r="D376" t="inlineStr"/>
+      <c r="D376" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E376" t="n">
         <v>35</v>
       </c>
@@ -7619,7 +7807,11 @@
           <t>November 9 - Line 3 (35)</t>
         </is>
       </c>
-      <c r="D377" t="inlineStr"/>
+      <c r="D377" t="inlineStr">
+        <is>
+          <t>Bobby Dinerstein</t>
+        </is>
+      </c>
       <c r="E377" t="n">
         <v>35</v>
       </c>
@@ -7640,7 +7832,7 @@
       </c>
       <c r="D378" t="inlineStr">
         <is>
-          <t>Yahrtzeit of Dave Szalavetz</t>
+          <t>Happy Birthday</t>
         </is>
       </c>
       <c r="E378" t="n">
@@ -7663,7 +7855,7 @@
       </c>
       <c r="D379" t="inlineStr">
         <is>
-          <t>Yitzchok b. Menachem Mendel HaKohen</t>
+          <t>Rivkah Leverton</t>
         </is>
       </c>
       <c r="E379" t="n">
@@ -7988,7 +8180,11 @@
           <t>November 13 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D396" t="inlineStr"/>
+      <c r="D396" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E396" t="n">
         <v>35</v>
       </c>
@@ -8007,7 +8203,11 @@
           <t>November 13 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D397" t="inlineStr"/>
+      <c r="D397" t="inlineStr">
+        <is>
+          <t>Rebbetzin Ruth Fisher</t>
+        </is>
+      </c>
       <c r="E397" t="n">
         <v>35</v>
       </c>
@@ -8026,7 +8226,11 @@
           <t>November 13 - Line 4 (25)</t>
         </is>
       </c>
-      <c r="D398" t="inlineStr"/>
+      <c r="D398" t="inlineStr">
+        <is>
+          <t>Happy Birthday</t>
+        </is>
+      </c>
       <c r="E398" t="n">
         <v>25</v>
       </c>
@@ -8045,7 +8249,11 @@
           <t>November 13 - Line 3 (35)</t>
         </is>
       </c>
-      <c r="D399" t="inlineStr"/>
+      <c r="D399" t="inlineStr">
+        <is>
+          <t>Aliza Leverton</t>
+        </is>
+      </c>
       <c r="E399" t="n">
         <v>35</v>
       </c>
@@ -8273,11 +8481,7 @@
           <t>November 15 - Line 3 (35)</t>
         </is>
       </c>
-      <c r="D411" t="inlineStr">
-        <is>
-          <t>Happy Birthday Leiba (Lara)</t>
-        </is>
-      </c>
+      <c r="D411" t="inlineStr"/>
       <c r="E411" t="n">
         <v>35</v>
       </c>
@@ -8315,11 +8519,7 @@
           <t>November 15 - Line 1 (35)</t>
         </is>
       </c>
-      <c r="D413" t="inlineStr">
-        <is>
-          <t>Yahrtzeit of Eda Tarlo</t>
-        </is>
-      </c>
+      <c r="D413" t="inlineStr"/>
       <c r="E413" t="n">
         <v>35</v>
       </c>
@@ -8414,11 +8614,7 @@
           <t>November 16 - Line 2 (35)</t>
         </is>
       </c>
-      <c r="D418" t="inlineStr">
-        <is>
-          <t>Yahrtzeit of Arnold Harold Aaron</t>
-        </is>
-      </c>
+      <c r="D418" t="inlineStr"/>
       <c r="E418" t="n">
         <v>35</v>
       </c>
@@ -8437,11 +8633,7 @@
           <t>November 16 - Line 1 (35)</t>
         </is>
       </c>
-      <c r="D419" t="inlineStr">
-        <is>
-          <t>Aaron Ben Dov</t>
-        </is>
-      </c>
+      <c r="D419" t="inlineStr"/>
       <c r="E419" t="n">
         <v>35</v>
       </c>
@@ -8574,7 +8766,11 @@
           <t>November 18 - Line 5 (25)</t>
         </is>
       </c>
-      <c r="D426" t="inlineStr"/>
+      <c r="D426" t="inlineStr">
+        <is>
+          <t>Fanny Medina</t>
+        </is>
+      </c>
       <c r="E426" t="n">
         <v>25</v>
       </c>
@@ -8650,11 +8846,7 @@
           <t>November 18 - Line 1 (35)</t>
         </is>
       </c>
-      <c r="D430" t="inlineStr">
-        <is>
-          <t>Happy Birthday Noam</t>
-        </is>
-      </c>
+      <c r="D430" t="inlineStr"/>
       <c r="E430" t="n">
         <v>35</v>
       </c>
@@ -8787,7 +8979,11 @@
           <t>November 20 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D437" t="inlineStr"/>
+      <c r="D437" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E437" t="n">
         <v>35</v>
       </c>
@@ -8806,7 +9002,11 @@
           <t>November 20 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D438" t="inlineStr"/>
+      <c r="D438" t="inlineStr">
+        <is>
+          <t>Sarah Felber</t>
+        </is>
+      </c>
       <c r="E438" t="n">
         <v>35</v>
       </c>
@@ -8901,7 +9101,11 @@
           <t>November 21 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D443" t="inlineStr"/>
+      <c r="D443" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E443" t="n">
         <v>35</v>
       </c>
@@ -8920,7 +9124,11 @@
           <t>November 21 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D444" t="inlineStr"/>
+      <c r="D444" t="inlineStr">
+        <is>
+          <t>Leonard Cagan</t>
+        </is>
+      </c>
       <c r="E444" t="n">
         <v>35</v>
       </c>
@@ -9243,7 +9451,11 @@
           <t>November 24 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D461" t="inlineStr"/>
+      <c r="D461" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E461" t="n">
         <v>35</v>
       </c>
@@ -9262,7 +9474,11 @@
           <t>November 24 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D462" t="inlineStr"/>
+      <c r="D462" t="inlineStr">
+        <is>
+          <t>Selma Yellin</t>
+        </is>
+      </c>
       <c r="E462" t="n">
         <v>35</v>
       </c>
@@ -9281,7 +9497,11 @@
           <t>November 24 - Line 4 (35)</t>
         </is>
       </c>
-      <c r="D463" t="inlineStr"/>
+      <c r="D463" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E463" t="n">
         <v>35</v>
       </c>
@@ -9300,7 +9520,11 @@
           <t>November 24 - Line 3 (35)</t>
         </is>
       </c>
-      <c r="D464" t="inlineStr"/>
+      <c r="D464" t="inlineStr">
+        <is>
+          <t>Lois Saltin</t>
+        </is>
+      </c>
       <c r="E464" t="n">
         <v>35</v>
       </c>
@@ -10421,11 +10645,7 @@
           <t>December 4 - Line 1 (35)</t>
         </is>
       </c>
-      <c r="D523" t="inlineStr">
-        <is>
-          <t>Happy Birthday Simcha Chaim (Sam)</t>
-        </is>
-      </c>
+      <c r="D523" t="inlineStr"/>
       <c r="E523" t="n">
         <v>35</v>
       </c>
@@ -10444,7 +10664,11 @@
           <t>December 5 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D524" t="inlineStr"/>
+      <c r="D524" t="inlineStr">
+        <is>
+          <t>Happy Birthday</t>
+        </is>
+      </c>
       <c r="E524" t="n">
         <v>35</v>
       </c>
@@ -10463,7 +10687,11 @@
           <t>December 5 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D525" t="inlineStr"/>
+      <c r="D525" t="inlineStr">
+        <is>
+          <t>Esther Kalif</t>
+        </is>
+      </c>
       <c r="E525" t="n">
         <v>35</v>
       </c>
@@ -10482,7 +10710,11 @@
           <t>December 5 - Line 4 (35)</t>
         </is>
       </c>
-      <c r="D526" t="inlineStr"/>
+      <c r="D526" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E526" t="n">
         <v>35</v>
       </c>
@@ -10501,7 +10733,11 @@
           <t>December 5 - Line 3 (35)</t>
         </is>
       </c>
-      <c r="D527" t="inlineStr"/>
+      <c r="D527" t="inlineStr">
+        <is>
+          <t>Alfred Sapolnick</t>
+        </is>
+      </c>
       <c r="E527" t="n">
         <v>35</v>
       </c>
@@ -11280,7 +11516,11 @@
           <t>December 16 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D568" t="inlineStr"/>
+      <c r="D568" t="inlineStr">
+        <is>
+          <t>Helene Benaroch de Natera</t>
+        </is>
+      </c>
       <c r="E568" t="n">
         <v>35</v>
       </c>
@@ -12135,7 +12375,11 @@
           <t>December 25 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D613" t="inlineStr"/>
+      <c r="D613" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E613" t="n">
         <v>35</v>
       </c>
@@ -12154,7 +12398,11 @@
           <t>December 25 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D614" t="inlineStr"/>
+      <c r="D614" t="inlineStr">
+        <is>
+          <t>Amnum Ben Ruben Moshiyakhov</t>
+        </is>
+      </c>
       <c r="E614" t="n">
         <v>35</v>
       </c>
@@ -12173,7 +12421,11 @@
           <t>December 25 - Line 4 (35)</t>
         </is>
       </c>
-      <c r="D615" t="inlineStr"/>
+      <c r="D615" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E615" t="n">
         <v>35</v>
       </c>
@@ -12192,7 +12444,11 @@
           <t>December 25 - Line 3 (35)</t>
         </is>
       </c>
-      <c r="D616" t="inlineStr"/>
+      <c r="D616" t="inlineStr">
+        <is>
+          <t>Ann Kaplowitz</t>
+        </is>
+      </c>
       <c r="E616" t="n">
         <v>35</v>
       </c>
@@ -13161,11 +13417,7 @@
           <t>January 3 - Line 1 (35)</t>
         </is>
       </c>
-      <c r="D667" t="inlineStr">
-        <is>
-          <t>Yahrtzeit Nanette Ogulnik</t>
-        </is>
-      </c>
+      <c r="D667" t="inlineStr"/>
       <c r="E667" t="n">
         <v>35</v>
       </c>
@@ -13412,7 +13664,11 @@
           <t>January 6 - Line 4 (35)</t>
         </is>
       </c>
-      <c r="D680" t="inlineStr"/>
+      <c r="D680" t="inlineStr">
+        <is>
+          <t>Happy Birthday</t>
+        </is>
+      </c>
       <c r="E680" t="n">
         <v>35</v>
       </c>
@@ -13431,7 +13687,11 @@
           <t>January 6 - Line 3 (35)</t>
         </is>
       </c>
-      <c r="D681" t="inlineStr"/>
+      <c r="D681" t="inlineStr">
+        <is>
+          <t>Avraham Leverton</t>
+        </is>
+      </c>
       <c r="E681" t="n">
         <v>35</v>
       </c>
@@ -13602,7 +13862,11 @@
           <t>January 8 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D690" t="inlineStr"/>
+      <c r="D690" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E690" t="n">
         <v>35</v>
       </c>
@@ -13621,7 +13885,11 @@
           <t>January 8 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D691" t="inlineStr"/>
+      <c r="D691" t="inlineStr">
+        <is>
+          <t>Julius Bloom</t>
+        </is>
+      </c>
       <c r="E691" t="n">
         <v>35</v>
       </c>
@@ -13640,7 +13908,11 @@
           <t>January 8 - Line 4 (35)</t>
         </is>
       </c>
-      <c r="D692" t="inlineStr"/>
+      <c r="D692" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E692" t="n">
         <v>35</v>
       </c>
@@ -13659,7 +13931,11 @@
           <t>January 8 - Line 3 (35)</t>
         </is>
       </c>
-      <c r="D693" t="inlineStr"/>
+      <c r="D693" t="inlineStr">
+        <is>
+          <t>Barry Weissman</t>
+        </is>
+      </c>
       <c r="E693" t="n">
         <v>35</v>
       </c>
@@ -13944,7 +14220,11 @@
           <t>January 11 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D708" t="inlineStr"/>
+      <c r="D708" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E708" t="n">
         <v>35</v>
       </c>
@@ -13963,7 +14243,11 @@
           <t>January 11 - Line 4 (35)</t>
         </is>
       </c>
-      <c r="D709" t="inlineStr"/>
+      <c r="D709" t="inlineStr">
+        <is>
+          <t>John J. Gavula</t>
+        </is>
+      </c>
       <c r="E709" t="n">
         <v>35</v>
       </c>
@@ -13982,7 +14266,11 @@
           <t>January 11 - Line 3 (35)</t>
         </is>
       </c>
-      <c r="D710" t="inlineStr"/>
+      <c r="D710" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E710" t="n">
         <v>35</v>
       </c>
@@ -14001,7 +14289,11 @@
           <t>January 11 - Line 2 (35)</t>
         </is>
       </c>
-      <c r="D711" t="inlineStr"/>
+      <c r="D711" t="inlineStr">
+        <is>
+          <t>Abraham Felber</t>
+        </is>
+      </c>
       <c r="E711" t="n">
         <v>35</v>
       </c>
@@ -14020,11 +14312,7 @@
           <t>January 11 - Line 1 (35)</t>
         </is>
       </c>
-      <c r="D712" t="inlineStr">
-        <is>
-          <t>Yahrtzeit of Yisrael (Richard) King</t>
-        </is>
-      </c>
+      <c r="D712" t="inlineStr"/>
       <c r="E712" t="n">
         <v>35</v>
       </c>
@@ -14157,7 +14445,11 @@
           <t>January 13 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D719" t="inlineStr"/>
+      <c r="D719" t="inlineStr">
+        <is>
+          <t>Pearl Granoff</t>
+        </is>
+      </c>
       <c r="E719" t="n">
         <v>35</v>
       </c>
@@ -14366,7 +14658,11 @@
           <t>January 15 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D730" t="inlineStr"/>
+      <c r="D730" t="inlineStr">
+        <is>
+          <t>Happy Birthday</t>
+        </is>
+      </c>
       <c r="E730" t="n">
         <v>35</v>
       </c>
@@ -14385,7 +14681,11 @@
           <t>January 15 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D731" t="inlineStr"/>
+      <c r="D731" t="inlineStr">
+        <is>
+          <t>Aaron Budanitsky</t>
+        </is>
+      </c>
       <c r="E731" t="n">
         <v>35</v>
       </c>
@@ -14499,7 +14799,11 @@
           <t>January 16 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D737" t="inlineStr"/>
+      <c r="D737" t="inlineStr">
+        <is>
+          <t>Happy Birthday</t>
+        </is>
+      </c>
       <c r="E737" t="n">
         <v>35</v>
       </c>
@@ -14518,7 +14822,11 @@
           <t>January 16 - Line 4 (35)</t>
         </is>
       </c>
-      <c r="D738" t="inlineStr"/>
+      <c r="D738" t="inlineStr">
+        <is>
+          <t>Mark Safran</t>
+        </is>
+      </c>
       <c r="E738" t="n">
         <v>35</v>
       </c>
@@ -14708,7 +15016,11 @@
           <t>January 18 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D748" t="inlineStr"/>
+      <c r="D748" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E748" t="n">
         <v>35</v>
       </c>
@@ -14727,7 +15039,11 @@
           <t>January 18 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D749" t="inlineStr"/>
+      <c r="D749" t="inlineStr">
+        <is>
+          <t>Tatiana Friedman</t>
+        </is>
+      </c>
       <c r="E749" t="n">
         <v>35</v>
       </c>
@@ -14898,11 +15214,7 @@
           <t>January 19 - Line 2 (35)</t>
         </is>
       </c>
-      <c r="D758" t="inlineStr">
-        <is>
-          <t>Yahrtzeit of Mayer Ginsberg</t>
-        </is>
-      </c>
+      <c r="D758" t="inlineStr"/>
       <c r="E758" t="n">
         <v>35</v>
       </c>
@@ -14921,11 +15233,7 @@
           <t>January 19 - Line 1 (35)</t>
         </is>
       </c>
-      <c r="D759" t="inlineStr">
-        <is>
-          <t>Eliyahu Mayer ben Tzvi</t>
-        </is>
-      </c>
+      <c r="D759" t="inlineStr"/>
       <c r="E759" t="n">
         <v>35</v>
       </c>
@@ -15153,7 +15461,11 @@
           <t>January 22 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D771" t="inlineStr"/>
+      <c r="D771" t="inlineStr">
+        <is>
+          <t>Anniversary</t>
+        </is>
+      </c>
       <c r="E771" t="n">
         <v>35</v>
       </c>
@@ -15172,7 +15484,11 @@
           <t>January 22 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D772" t="inlineStr"/>
+      <c r="D772" t="inlineStr">
+        <is>
+          <t>Sholom &amp; Aliza Leverton</t>
+        </is>
+      </c>
       <c r="E772" t="n">
         <v>35</v>
       </c>
@@ -15362,11 +15678,7 @@
           <t>January 23 - Line 1 (35)</t>
         </is>
       </c>
-      <c r="D782" t="inlineStr">
-        <is>
-          <t>Happy Birthday Hanna Houdayer</t>
-        </is>
-      </c>
+      <c r="D782" t="inlineStr"/>
       <c r="E782" t="n">
         <v>35</v>
       </c>
@@ -15385,7 +15697,11 @@
           <t>January 24 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D783" t="inlineStr"/>
+      <c r="D783" t="inlineStr">
+        <is>
+          <t>Happy Birthday</t>
+        </is>
+      </c>
       <c r="E783" t="n">
         <v>35</v>
       </c>
@@ -15404,7 +15720,11 @@
           <t>January 24 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D784" t="inlineStr"/>
+      <c r="D784" t="inlineStr">
+        <is>
+          <t>Amy Abayev</t>
+        </is>
+      </c>
       <c r="E784" t="n">
         <v>35</v>
       </c>
@@ -15461,11 +15781,7 @@
           <t>January 24 - Line 2 (35)</t>
         </is>
       </c>
-      <c r="D787" t="inlineStr">
-        <is>
-          <t>Yahrtzeit of Herbert Rubin</t>
-        </is>
-      </c>
+      <c r="D787" t="inlineStr"/>
       <c r="E787" t="n">
         <v>35</v>
       </c>
@@ -15484,11 +15800,7 @@
           <t>January 24 - Line 1 (35)</t>
         </is>
       </c>
-      <c r="D788" t="inlineStr">
-        <is>
-          <t>Chaim ben Dovid Hakohen</t>
-        </is>
-      </c>
+      <c r="D788" t="inlineStr"/>
       <c r="E788" t="n">
         <v>35</v>
       </c>
@@ -15716,11 +16028,7 @@
           <t>January 26 - Line 1 (35)</t>
         </is>
       </c>
-      <c r="D800" t="inlineStr">
-        <is>
-          <t>Happy Birthday Ruth Doerfler</t>
-        </is>
-      </c>
+      <c r="D800" t="inlineStr"/>
       <c r="E800" t="n">
         <v>35</v>
       </c>
@@ -15929,7 +16237,11 @@
           <t>January 29 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D811" t="inlineStr"/>
+      <c r="D811" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E811" t="n">
         <v>35</v>
       </c>
@@ -15948,7 +16260,11 @@
           <t>January 29 - Line 4 (35)</t>
         </is>
       </c>
-      <c r="D812" t="inlineStr"/>
+      <c r="D812" t="inlineStr">
+        <is>
+          <t>Celia Golbert</t>
+        </is>
+      </c>
       <c r="E812" t="n">
         <v>35</v>
       </c>
@@ -16138,7 +16454,11 @@
           <t>January 31 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D822" t="inlineStr"/>
+      <c r="D822" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E822" t="n">
         <v>35</v>
       </c>
@@ -16157,7 +16477,11 @@
           <t>January 31 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D823" t="inlineStr"/>
+      <c r="D823" t="inlineStr">
+        <is>
+          <t>Bertha Shapiro</t>
+        </is>
+      </c>
       <c r="E823" t="n">
         <v>35</v>
       </c>
@@ -16233,11 +16557,7 @@
           <t>January 31 - Line 1 (35)</t>
         </is>
       </c>
-      <c r="D827" t="inlineStr">
-        <is>
-          <t>Happy Birthday Nathaniel Bendahan</t>
-        </is>
-      </c>
+      <c r="D827" t="inlineStr"/>
       <c r="E827" t="n">
         <v>35</v>
       </c>
@@ -16332,11 +16652,7 @@
           <t>February 1 - Line 2 (35)</t>
         </is>
       </c>
-      <c r="D832" t="inlineStr">
-        <is>
-          <t>Yahrtzeit of Joe Schlesinger</t>
-        </is>
-      </c>
+      <c r="D832" t="inlineStr"/>
       <c r="E832" t="n">
         <v>35</v>
       </c>
@@ -16355,11 +16671,7 @@
           <t>February 1 - Line 1 (35)</t>
         </is>
       </c>
-      <c r="D833" t="inlineStr">
-        <is>
-          <t>Yosef ben Yechiel</t>
-        </is>
-      </c>
+      <c r="D833" t="inlineStr"/>
       <c r="E833" t="n">
         <v>35</v>
       </c>
@@ -16568,7 +16880,11 @@
           <t>February 4 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D844" t="inlineStr"/>
+      <c r="D844" t="inlineStr">
+        <is>
+          <t>Happy Birthday</t>
+        </is>
+      </c>
       <c r="E844" t="n">
         <v>35</v>
       </c>
@@ -16587,7 +16903,11 @@
           <t>February 4 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D845" t="inlineStr"/>
+      <c r="D845" t="inlineStr">
+        <is>
+          <t>Toby Kane</t>
+        </is>
+      </c>
       <c r="E845" t="n">
         <v>35</v>
       </c>
@@ -16682,7 +17002,11 @@
           <t>February 5 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D850" t="inlineStr"/>
+      <c r="D850" t="inlineStr">
+        <is>
+          <t>Happy Birthday</t>
+        </is>
+      </c>
       <c r="E850" t="n">
         <v>35</v>
       </c>
@@ -16701,7 +17025,11 @@
           <t>February 5 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D851" t="inlineStr"/>
+      <c r="D851" t="inlineStr">
+        <is>
+          <t>Rebecca Bershad</t>
+        </is>
+      </c>
       <c r="E851" t="n">
         <v>35</v>
       </c>
@@ -17385,7 +17713,11 @@
           <t>February 12 - Line 6 (25)</t>
         </is>
       </c>
-      <c r="D887" t="inlineStr"/>
+      <c r="D887" t="inlineStr">
+        <is>
+          <t>Happy Birthday</t>
+        </is>
+      </c>
       <c r="E887" t="n">
         <v>25</v>
       </c>
@@ -17404,7 +17736,11 @@
           <t>February 12 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D888" t="inlineStr"/>
+      <c r="D888" t="inlineStr">
+        <is>
+          <t>Adam Bershad</t>
+        </is>
+      </c>
       <c r="E888" t="n">
         <v>35</v>
       </c>
@@ -17461,11 +17797,7 @@
           <t>February 12 - Line 2 (35)</t>
         </is>
       </c>
-      <c r="D891" t="inlineStr">
-        <is>
-          <t>Yahrtzeit of Grace Lassner</t>
-        </is>
-      </c>
+      <c r="D891" t="inlineStr"/>
       <c r="E891" t="n">
         <v>35</v>
       </c>
@@ -17484,11 +17816,7 @@
           <t>February 12 - Line 1 (35)</t>
         </is>
       </c>
-      <c r="D892" t="inlineStr">
-        <is>
-          <t>Gittel bas Aharon Tzvi</t>
-        </is>
-      </c>
+      <c r="D892" t="inlineStr"/>
       <c r="E892" t="n">
         <v>35</v>
       </c>
@@ -17621,7 +17949,11 @@
           <t>February 14 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D899" t="inlineStr"/>
+      <c r="D899" t="inlineStr">
+        <is>
+          <t>Happy Birthday</t>
+        </is>
+      </c>
       <c r="E899" t="n">
         <v>35</v>
       </c>
@@ -17640,7 +17972,11 @@
           <t>February 14 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D900" t="inlineStr"/>
+      <c r="D900" t="inlineStr">
+        <is>
+          <t>Aaron Abayev</t>
+        </is>
+      </c>
       <c r="E900" t="n">
         <v>35</v>
       </c>
@@ -18058,7 +18394,11 @@
           <t>February 18 - Line 6 (25)</t>
         </is>
       </c>
-      <c r="D922" t="inlineStr"/>
+      <c r="D922" t="inlineStr">
+        <is>
+          <t>Happy Anniversary</t>
+        </is>
+      </c>
       <c r="E922" t="n">
         <v>25</v>
       </c>
@@ -18077,7 +18417,11 @@
           <t>February 18 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D923" t="inlineStr"/>
+      <c r="D923" t="inlineStr">
+        <is>
+          <t>Enid &amp; William Weinstein</t>
+        </is>
+      </c>
       <c r="E923" t="n">
         <v>35</v>
       </c>
@@ -18096,7 +18440,11 @@
           <t>February 18 - Line 4 (35)</t>
         </is>
       </c>
-      <c r="D924" t="inlineStr"/>
+      <c r="D924" t="inlineStr">
+        <is>
+          <t>Happy Birthday</t>
+        </is>
+      </c>
       <c r="E924" t="n">
         <v>35</v>
       </c>
@@ -18115,7 +18463,11 @@
           <t>February 18 - Line 3 (25)</t>
         </is>
       </c>
-      <c r="D925" t="inlineStr"/>
+      <c r="D925" t="inlineStr">
+        <is>
+          <t>Hym Josef Ben Joshua</t>
+        </is>
+      </c>
       <c r="E925" t="n">
         <v>25</v>
       </c>
@@ -18172,7 +18524,11 @@
           <t>February 19 - Line 6 (25)</t>
         </is>
       </c>
-      <c r="D928" t="inlineStr"/>
+      <c r="D928" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E928" t="n">
         <v>25</v>
       </c>
@@ -18191,7 +18547,11 @@
           <t>February 19 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D929" t="inlineStr"/>
+      <c r="D929" t="inlineStr">
+        <is>
+          <t>Thomas Tanenhaus M.D.</t>
+        </is>
+      </c>
       <c r="E929" t="n">
         <v>35</v>
       </c>
@@ -18381,11 +18741,7 @@
           <t>February 20 - Line 1 (35)</t>
         </is>
       </c>
-      <c r="D939" t="inlineStr">
-        <is>
-          <t>Yahrtzeit of Isidore Echenberg</t>
-        </is>
-      </c>
+      <c r="D939" t="inlineStr"/>
       <c r="E939" t="n">
         <v>35</v>
       </c>
@@ -18746,7 +19102,11 @@
           <t>February 24 - Line 5 (25)</t>
         </is>
       </c>
-      <c r="D958" t="inlineStr"/>
+      <c r="D958" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E958" t="n">
         <v>25</v>
       </c>
@@ -18765,7 +19125,11 @@
           <t>February 24 - Line 4 (35)</t>
         </is>
       </c>
-      <c r="D959" t="inlineStr"/>
+      <c r="D959" t="inlineStr">
+        <is>
+          <t>Edna Hawkins</t>
+        </is>
+      </c>
       <c r="E959" t="n">
         <v>35</v>
       </c>
@@ -18955,7 +19319,11 @@
           <t>February 26 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D969" t="inlineStr"/>
+      <c r="D969" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E969" t="n">
         <v>35</v>
       </c>
@@ -18974,7 +19342,11 @@
           <t>February 26 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D970" t="inlineStr"/>
+      <c r="D970" t="inlineStr">
+        <is>
+          <t>Zvi Pomper</t>
+        </is>
+      </c>
       <c r="E970" t="n">
         <v>35</v>
       </c>
@@ -19126,7 +19498,11 @@
           <t>February 27 - Line 3 (35)</t>
         </is>
       </c>
-      <c r="D978" t="inlineStr"/>
+      <c r="D978" t="inlineStr">
+        <is>
+          <t>Happy Birthday</t>
+        </is>
+      </c>
       <c r="E978" t="n">
         <v>35</v>
       </c>
@@ -19145,7 +19521,11 @@
           <t>February 27 - Line 2 (35)</t>
         </is>
       </c>
-      <c r="D979" t="inlineStr"/>
+      <c r="D979" t="inlineStr">
+        <is>
+          <t>Eliezer Lior Ben Joshua</t>
+        </is>
+      </c>
       <c r="E979" t="n">
         <v>35</v>
       </c>
@@ -19166,7 +19546,7 @@
       </c>
       <c r="D980" t="inlineStr">
         <is>
-          <t>Happy Birthday Yeshayahu (Jack)</t>
+          <t>Yahrtzeit Jacob Golbert</t>
         </is>
       </c>
       <c r="E980" t="n">
@@ -19187,7 +19567,11 @@
           <t>February 28 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D981" t="inlineStr"/>
+      <c r="D981" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E981" t="n">
         <v>35</v>
       </c>
@@ -19206,7 +19590,11 @@
           <t>February 28 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D982" t="inlineStr"/>
+      <c r="D982" t="inlineStr">
+        <is>
+          <t>Mordechai son of Dov Bear</t>
+        </is>
+      </c>
       <c r="E982" t="n">
         <v>35</v>
       </c>
@@ -19301,7 +19689,11 @@
           <t>February 29 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D987" t="inlineStr"/>
+      <c r="D987" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E987" t="n">
         <v>35</v>
       </c>
@@ -19320,7 +19712,11 @@
           <t>February 29 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D988" t="inlineStr"/>
+      <c r="D988" t="inlineStr">
+        <is>
+          <t>Tillie Shapiro</t>
+        </is>
+      </c>
       <c r="E988" t="n">
         <v>35</v>
       </c>
@@ -19339,7 +19735,11 @@
           <t>February 29 - Line 4 (35)</t>
         </is>
       </c>
-      <c r="D989" t="inlineStr"/>
+      <c r="D989" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E989" t="n">
         <v>35</v>
       </c>
@@ -19358,7 +19758,11 @@
           <t>February 29 - Line 3 (35)</t>
         </is>
       </c>
-      <c r="D990" t="inlineStr"/>
+      <c r="D990" t="inlineStr">
+        <is>
+          <t>Edward Kempner</t>
+        </is>
+      </c>
       <c r="E990" t="n">
         <v>35</v>
       </c>
@@ -19624,7 +20028,11 @@
           <t>March 3 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D1004" t="inlineStr"/>
+      <c r="D1004" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E1004" t="n">
         <v>35</v>
       </c>
@@ -19643,7 +20051,11 @@
           <t>March 3 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D1005" t="inlineStr"/>
+      <c r="D1005" t="inlineStr">
+        <is>
+          <t>Irving Granoff</t>
+        </is>
+      </c>
       <c r="E1005" t="n">
         <v>35</v>
       </c>
@@ -19966,7 +20378,11 @@
           <t>March 6 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D1022" t="inlineStr"/>
+      <c r="D1022" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E1022" t="n">
         <v>35</v>
       </c>
@@ -19985,7 +20401,11 @@
           <t>March 6 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D1023" t="inlineStr"/>
+      <c r="D1023" t="inlineStr">
+        <is>
+          <t>Esther Wishnev</t>
+        </is>
+      </c>
       <c r="E1023" t="n">
         <v>35</v>
       </c>
@@ -20422,7 +20842,11 @@
           <t>March 11 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D1046" t="inlineStr"/>
+      <c r="D1046" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E1046" t="n">
         <v>35</v>
       </c>
@@ -20441,7 +20865,11 @@
           <t>March 11 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D1047" t="inlineStr"/>
+      <c r="D1047" t="inlineStr">
+        <is>
+          <t>Rose Kempner</t>
+        </is>
+      </c>
       <c r="E1047" t="n">
         <v>35</v>
       </c>
@@ -20650,7 +21078,11 @@
           <t>March 13 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D1058" t="inlineStr"/>
+      <c r="D1058" t="inlineStr">
+        <is>
+          <t>Happy Birthday</t>
+        </is>
+      </c>
       <c r="E1058" t="n">
         <v>35</v>
       </c>
@@ -20669,7 +21101,11 @@
           <t>March 13 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D1059" t="inlineStr"/>
+      <c r="D1059" t="inlineStr">
+        <is>
+          <t>Adam Bershad</t>
+        </is>
+      </c>
       <c r="E1059" t="n">
         <v>35</v>
       </c>
@@ -20726,11 +21162,7 @@
           <t>March 13 - Line 2 (35)</t>
         </is>
       </c>
-      <c r="D1062" t="inlineStr">
-        <is>
-          <t>Yahrtzeit of Grace Lassner</t>
-        </is>
-      </c>
+      <c r="D1062" t="inlineStr"/>
       <c r="E1062" t="n">
         <v>35</v>
       </c>
@@ -20749,11 +21181,7 @@
           <t>March 13 - Line 1 (35)</t>
         </is>
       </c>
-      <c r="D1063" t="inlineStr">
-        <is>
-          <t>Gittel bas Aharon Tzvi</t>
-        </is>
-      </c>
+      <c r="D1063" t="inlineStr"/>
       <c r="E1063" t="n">
         <v>35</v>
       </c>
@@ -20886,7 +21314,11 @@
           <t>March 15 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D1070" t="inlineStr"/>
+      <c r="D1070" t="inlineStr">
+        <is>
+          <t>Happy Birthday</t>
+        </is>
+      </c>
       <c r="E1070" t="n">
         <v>35</v>
       </c>
@@ -20905,7 +21337,11 @@
           <t>March 15 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D1071" t="inlineStr"/>
+      <c r="D1071" t="inlineStr">
+        <is>
+          <t>Aaron Abayev</t>
+        </is>
+      </c>
       <c r="E1071" t="n">
         <v>35</v>
       </c>
@@ -21323,7 +21759,11 @@
           <t>March 19 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D1093" t="inlineStr"/>
+      <c r="D1093" t="inlineStr">
+        <is>
+          <t>Happy Anniversary</t>
+        </is>
+      </c>
       <c r="E1093" t="n">
         <v>35</v>
       </c>
@@ -21342,7 +21782,11 @@
           <t>March 19 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D1094" t="inlineStr"/>
+      <c r="D1094" t="inlineStr">
+        <is>
+          <t>Enid &amp; William Weinstein</t>
+        </is>
+      </c>
       <c r="E1094" t="n">
         <v>35</v>
       </c>
@@ -21361,7 +21805,11 @@
           <t>March 19 - Line 4 (35)</t>
         </is>
       </c>
-      <c r="D1095" t="inlineStr"/>
+      <c r="D1095" t="inlineStr">
+        <is>
+          <t>Happy Birthday</t>
+        </is>
+      </c>
       <c r="E1095" t="n">
         <v>35</v>
       </c>
@@ -21380,7 +21828,11 @@
           <t>March 19 - Line 3 (35)</t>
         </is>
       </c>
-      <c r="D1096" t="inlineStr"/>
+      <c r="D1096" t="inlineStr">
+        <is>
+          <t>Hym Josef Ben Joshua</t>
+        </is>
+      </c>
       <c r="E1096" t="n">
         <v>35</v>
       </c>
@@ -21437,7 +21889,11 @@
           <t>March 20 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D1099" t="inlineStr"/>
+      <c r="D1099" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E1099" t="n">
         <v>35</v>
       </c>
@@ -21456,7 +21912,11 @@
           <t>March 20 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D1100" t="inlineStr"/>
+      <c r="D1100" t="inlineStr">
+        <is>
+          <t>Thomas Tanenhaus M.D.</t>
+        </is>
+      </c>
       <c r="E1100" t="n">
         <v>35</v>
       </c>
@@ -21608,11 +22068,7 @@
           <t>March 21 - Line 1 (35)</t>
         </is>
       </c>
-      <c r="D1108" t="inlineStr">
-        <is>
-          <t>Yahrtzeit of Isidore Echenberg</t>
-        </is>
-      </c>
+      <c r="D1108" t="inlineStr"/>
       <c r="E1108" t="n">
         <v>35</v>
       </c>
@@ -21859,7 +22315,11 @@
           <t>March 25 - Line 5 (30)</t>
         </is>
       </c>
-      <c r="D1121" t="inlineStr"/>
+      <c r="D1121" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E1121" t="n">
         <v>30</v>
       </c>
@@ -21878,7 +22338,11 @@
           <t>March 25 - Line 4 (35)</t>
         </is>
       </c>
-      <c r="D1122" t="inlineStr"/>
+      <c r="D1122" t="inlineStr">
+        <is>
+          <t>Edna Hawkins</t>
+        </is>
+      </c>
       <c r="E1122" t="n">
         <v>35</v>
       </c>
@@ -22068,7 +22532,11 @@
           <t>March 27 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D1132" t="inlineStr"/>
+      <c r="D1132" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E1132" t="n">
         <v>35</v>
       </c>
@@ -22087,7 +22555,11 @@
           <t>March 27 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D1133" t="inlineStr"/>
+      <c r="D1133" t="inlineStr">
+        <is>
+          <t>Zvi Pomper</t>
+        </is>
+      </c>
       <c r="E1133" t="n">
         <v>35</v>
       </c>
@@ -22239,7 +22711,11 @@
           <t>March 28 - Line 3 (35)</t>
         </is>
       </c>
-      <c r="D1141" t="inlineStr"/>
+      <c r="D1141" t="inlineStr">
+        <is>
+          <t>Happy Birthday</t>
+        </is>
+      </c>
       <c r="E1141" t="n">
         <v>35</v>
       </c>
@@ -22258,7 +22734,11 @@
           <t>March 28 - Line 2 (35)</t>
         </is>
       </c>
-      <c r="D1142" t="inlineStr"/>
+      <c r="D1142" t="inlineStr">
+        <is>
+          <t>Eliezer Lior Ben Joshua</t>
+        </is>
+      </c>
       <c r="E1142" t="n">
         <v>35</v>
       </c>
@@ -22279,7 +22759,7 @@
       </c>
       <c r="D1143" t="inlineStr">
         <is>
-          <t>Happy Birthday Yeshayahu (Jack)</t>
+          <t>Yahrtzeit Jacob Golbert</t>
         </is>
       </c>
       <c r="E1143" t="n">
@@ -22300,7 +22780,11 @@
           <t>March 29 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D1144" t="inlineStr"/>
+      <c r="D1144" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E1144" t="n">
         <v>35</v>
       </c>
@@ -22319,7 +22803,11 @@
           <t>March 29 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D1145" t="inlineStr"/>
+      <c r="D1145" t="inlineStr">
+        <is>
+          <t>Mordechai son of Dov Bear</t>
+        </is>
+      </c>
       <c r="E1145" t="n">
         <v>35</v>
       </c>
@@ -22414,7 +22902,11 @@
           <t>March 30 - Line 3 (35)</t>
         </is>
       </c>
-      <c r="D1150" t="inlineStr"/>
+      <c r="D1150" t="inlineStr">
+        <is>
+          <t>Edward Kempner</t>
+        </is>
+      </c>
       <c r="E1150" t="n">
         <v>35</v>
       </c>
@@ -22604,7 +23096,11 @@
           <t>April 2 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D1160" t="inlineStr"/>
+      <c r="D1160" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E1160" t="n">
         <v>35</v>
       </c>
@@ -22623,7 +23119,11 @@
           <t>April 2 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D1161" t="inlineStr"/>
+      <c r="D1161" t="inlineStr">
+        <is>
+          <t>Irving Granoff</t>
+        </is>
+      </c>
       <c r="E1161" t="n">
         <v>35</v>
       </c>
@@ -22946,7 +23446,11 @@
           <t>April 5 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D1178" t="inlineStr"/>
+      <c r="D1178" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E1178" t="n">
         <v>35</v>
       </c>
@@ -22965,7 +23469,11 @@
           <t>April 5 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D1179" t="inlineStr"/>
+      <c r="D1179" t="inlineStr">
+        <is>
+          <t>Esther Wishnev</t>
+        </is>
+      </c>
       <c r="E1179" t="n">
         <v>35</v>
       </c>
@@ -23345,7 +23853,11 @@
           <t>April 9 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D1199" t="inlineStr"/>
+      <c r="D1199" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E1199" t="n">
         <v>35</v>
       </c>
@@ -23364,7 +23876,11 @@
           <t>April 9 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D1200" t="inlineStr"/>
+      <c r="D1200" t="inlineStr">
+        <is>
+          <t>Mina Kwitkin</t>
+        </is>
+      </c>
       <c r="E1200" t="n">
         <v>35</v>
       </c>
@@ -23592,7 +24108,11 @@
           <t>April 11 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D1212" t="inlineStr"/>
+      <c r="D1212" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E1212" t="n">
         <v>35</v>
       </c>
@@ -23611,7 +24131,11 @@
           <t>April 11 - Line 4 (35)</t>
         </is>
       </c>
-      <c r="D1213" t="inlineStr"/>
+      <c r="D1213" t="inlineStr">
+        <is>
+          <t>Miriam Warshawsky</t>
+        </is>
+      </c>
       <c r="E1213" t="n">
         <v>35</v>
       </c>
@@ -24466,7 +24990,11 @@
           <t>April 19 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D1258" t="inlineStr"/>
+      <c r="D1258" t="inlineStr">
+        <is>
+          <t>Anniversary</t>
+        </is>
+      </c>
       <c r="E1258" t="n">
         <v>35</v>
       </c>
@@ -24485,7 +25013,11 @@
           <t>April 19 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D1259" t="inlineStr"/>
+      <c r="D1259" t="inlineStr">
+        <is>
+          <t>Mark &amp; Kathryn Safran</t>
+        </is>
+      </c>
       <c r="E1259" t="n">
         <v>35</v>
       </c>
@@ -24770,7 +25302,11 @@
           <t>April 22 - Line 2 (35)</t>
         </is>
       </c>
-      <c r="D1274" t="inlineStr"/>
+      <c r="D1274" t="inlineStr">
+        <is>
+          <t>Debbie Goldberg Simmins</t>
+        </is>
+      </c>
       <c r="E1274" t="n">
         <v>35</v>
       </c>
@@ -24865,7 +25401,11 @@
           <t>April 24 - Line 3 (35)</t>
         </is>
       </c>
-      <c r="D1279" t="inlineStr"/>
+      <c r="D1279" t="inlineStr">
+        <is>
+          <t>Happy Birthday</t>
+        </is>
+      </c>
       <c r="E1279" t="n">
         <v>35</v>
       </c>
@@ -24884,7 +25424,11 @@
           <t>April 24 - Line 2 (35)</t>
         </is>
       </c>
-      <c r="D1280" t="inlineStr"/>
+      <c r="D1280" t="inlineStr">
+        <is>
+          <t>Annakah Smolensky</t>
+        </is>
+      </c>
       <c r="E1280" t="n">
         <v>35</v>
       </c>
@@ -25074,11 +25618,7 @@
           <t>April 27 - Line 2 (35)</t>
         </is>
       </c>
-      <c r="D1290" t="inlineStr">
-        <is>
-          <t>Happy Birthday</t>
-        </is>
-      </c>
+      <c r="D1290" t="inlineStr"/>
       <c r="E1290" t="n">
         <v>35</v>
       </c>
@@ -25097,11 +25637,7 @@
           <t>April 27 - Line 1 (35)</t>
         </is>
       </c>
-      <c r="D1291" t="inlineStr">
-        <is>
-          <t>Sarah (Caroline) Amzallag</t>
-        </is>
-      </c>
+      <c r="D1291" t="inlineStr"/>
       <c r="E1291" t="n">
         <v>35</v>
       </c>
@@ -25139,7 +25675,11 @@
           <t>April 28 - Line 2 (35)</t>
         </is>
       </c>
-      <c r="D1293" t="inlineStr"/>
+      <c r="D1293" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E1293" t="n">
         <v>35</v>
       </c>
@@ -25158,7 +25698,11 @@
           <t>April 28 - Line 1 (35)</t>
         </is>
       </c>
-      <c r="D1294" t="inlineStr"/>
+      <c r="D1294" t="inlineStr">
+        <is>
+          <t>Rabbi Mordechai Fisher</t>
+        </is>
+      </c>
       <c r="E1294" t="n">
         <v>35</v>
       </c>
@@ -25196,11 +25740,7 @@
           <t>April 29 - Line 2 (35)</t>
         </is>
       </c>
-      <c r="D1296" t="inlineStr">
-        <is>
-          <t>Happy Birthday</t>
-        </is>
-      </c>
+      <c r="D1296" t="inlineStr"/>
       <c r="E1296" t="n">
         <v>35</v>
       </c>
@@ -25219,11 +25759,7 @@
           <t>April 29 - Line 1 (35)</t>
         </is>
       </c>
-      <c r="D1297" t="inlineStr">
-        <is>
-          <t>Dr. Shlomo (Shawn) Cohen</t>
-        </is>
-      </c>
+      <c r="D1297" t="inlineStr"/>
       <c r="E1297" t="n">
         <v>35</v>
       </c>
@@ -25983,7 +26519,11 @@
           <t>May 8 - Line 3 (35)</t>
         </is>
       </c>
-      <c r="D1337" t="inlineStr"/>
+      <c r="D1337" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E1337" t="n">
         <v>35</v>
       </c>
@@ -26002,7 +26542,11 @@
           <t>May 8 - Line 2 (35)</t>
         </is>
       </c>
-      <c r="D1338" t="inlineStr"/>
+      <c r="D1338" t="inlineStr">
+        <is>
+          <t>Shoshana Daughter of Chaya</t>
+        </is>
+      </c>
       <c r="E1338" t="n">
         <v>35</v>
       </c>
@@ -26021,7 +26565,11 @@
           <t>May 8 - Line 1 (35)</t>
         </is>
       </c>
-      <c r="D1339" t="inlineStr"/>
+      <c r="D1339" t="inlineStr">
+        <is>
+          <t>Anniversary Bob &amp; Helen Wishnev</t>
+        </is>
+      </c>
       <c r="E1339" t="n">
         <v>35</v>
       </c>
@@ -26192,7 +26740,11 @@
           <t>May 10 - Line 1 (35)</t>
         </is>
       </c>
-      <c r="D1348" t="inlineStr"/>
+      <c r="D1348" t="inlineStr">
+        <is>
+          <t>Happy Birthday Rahm Kalif</t>
+        </is>
+      </c>
       <c r="E1348" t="n">
         <v>35</v>
       </c>
@@ -26439,11 +26991,7 @@
           <t>May 13 - Line 2 (35)</t>
         </is>
       </c>
-      <c r="D1361" t="inlineStr">
-        <is>
-          <t>Yahrtzeit of Lyla Rapkin</t>
-        </is>
-      </c>
+      <c r="D1361" t="inlineStr"/>
       <c r="E1361" t="n">
         <v>35</v>
       </c>
@@ -26462,11 +27010,7 @@
           <t>May 13 - Line 1 (35)</t>
         </is>
       </c>
-      <c r="D1362" t="inlineStr">
-        <is>
-          <t>Leah bas Aryeh Leib</t>
-        </is>
-      </c>
+      <c r="D1362" t="inlineStr"/>
       <c r="E1362" t="n">
         <v>35</v>
       </c>
@@ -26485,7 +27029,11 @@
           <t>May 14 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D1363" t="inlineStr"/>
+      <c r="D1363" t="inlineStr">
+        <is>
+          <t>Happy Birthday</t>
+        </is>
+      </c>
       <c r="E1363" t="n">
         <v>35</v>
       </c>
@@ -26504,7 +27052,11 @@
           <t>May 14 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D1364" t="inlineStr"/>
+      <c r="D1364" t="inlineStr">
+        <is>
+          <t>Matan Gavriel Kalif</t>
+        </is>
+      </c>
       <c r="E1364" t="n">
         <v>35</v>
       </c>
@@ -26561,11 +27113,7 @@
           <t>May 14 - Line 2 (35)</t>
         </is>
       </c>
-      <c r="D1367" t="inlineStr">
-        <is>
-          <t>Yahrtzeit of Mortimer Vineberg</t>
-        </is>
-      </c>
+      <c r="D1367" t="inlineStr"/>
       <c r="E1367" t="n">
         <v>35</v>
       </c>
@@ -26584,11 +27132,7 @@
           <t>May 14 - Line 1 (35)</t>
         </is>
       </c>
-      <c r="D1368" t="inlineStr">
-        <is>
-          <t>Mordechai ben Shmuel Avraham</t>
-        </is>
-      </c>
+      <c r="D1368" t="inlineStr"/>
       <c r="E1368" t="n">
         <v>35</v>
       </c>
@@ -27063,11 +27607,7 @@
           <t>May 19 - Line 2 (35)</t>
         </is>
       </c>
-      <c r="D1393" t="inlineStr">
-        <is>
-          <t>Yahrtzeit of Sidney Morris Copoloff</t>
-        </is>
-      </c>
+      <c r="D1393" t="inlineStr"/>
       <c r="E1393" t="n">
         <v>35</v>
       </c>
@@ -27086,11 +27626,7 @@
           <t xml:space="preserve">May 19 - Line 1 (35) </t>
         </is>
       </c>
-      <c r="D1394" t="inlineStr">
-        <is>
-          <t>Shlomo Moshe ben Refoel Tzvi</t>
-        </is>
-      </c>
+      <c r="D1394" t="inlineStr"/>
       <c r="E1394" t="n">
         <v>35</v>
       </c>
@@ -27109,7 +27645,11 @@
           <t>May 20 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D1395" t="inlineStr"/>
+      <c r="D1395" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E1395" t="n">
         <v>35</v>
       </c>
@@ -27128,7 +27668,11 @@
           <t>May 20 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D1396" t="inlineStr"/>
+      <c r="D1396" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rahma Sadoun </t>
+        </is>
+      </c>
       <c r="E1396" t="n">
         <v>35</v>
       </c>
@@ -27527,7 +28071,11 @@
           <t>May 24 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D1417" t="inlineStr"/>
+      <c r="D1417" t="inlineStr">
+        <is>
+          <t>Albert Shapiro</t>
+        </is>
+      </c>
       <c r="E1417" t="n">
         <v>35</v>
       </c>
@@ -27907,7 +28455,11 @@
           <t>May 28 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D1437" t="inlineStr"/>
+      <c r="D1437" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E1437" t="n">
         <v>35</v>
       </c>
@@ -27926,7 +28478,11 @@
           <t>May 28 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D1438" t="inlineStr"/>
+      <c r="D1438" t="inlineStr">
+        <is>
+          <t>Max Goldfarb</t>
+        </is>
+      </c>
       <c r="E1438" t="n">
         <v>35</v>
       </c>
@@ -28040,7 +28596,11 @@
           <t>May 29 - Line 5 (25)</t>
         </is>
       </c>
-      <c r="D1444" t="inlineStr"/>
+      <c r="D1444" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E1444" t="n">
         <v>25</v>
       </c>
@@ -28059,7 +28619,11 @@
           <t>May 29 - Line 4 (25)</t>
         </is>
       </c>
-      <c r="D1445" t="inlineStr"/>
+      <c r="D1445" t="inlineStr">
+        <is>
+          <t>Marvin Tanenhaus</t>
+        </is>
+      </c>
       <c r="E1445" t="n">
         <v>25</v>
       </c>
@@ -28192,7 +28756,11 @@
           <t>May 30 - Line 3 (35)</t>
         </is>
       </c>
-      <c r="D1452" t="inlineStr"/>
+      <c r="D1452" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E1452" t="n">
         <v>35</v>
       </c>
@@ -28211,7 +28779,11 @@
           <t>May 30 - Line 2 (35)</t>
         </is>
       </c>
-      <c r="D1453" t="inlineStr"/>
+      <c r="D1453" t="inlineStr">
+        <is>
+          <t>Herman Yellin</t>
+        </is>
+      </c>
       <c r="E1453" t="n">
         <v>35</v>
       </c>
@@ -28458,11 +29030,7 @@
           <t>June 2 - Line 2 (35)</t>
         </is>
       </c>
-      <c r="D1466" t="inlineStr">
-        <is>
-          <t>Yahtzeit of Mark Niloff</t>
-        </is>
-      </c>
+      <c r="D1466" t="inlineStr"/>
       <c r="E1466" t="n">
         <v>35</v>
       </c>
@@ -28481,11 +29049,7 @@
           <t>June 2 - Line 1 (35)</t>
         </is>
       </c>
-      <c r="D1467" t="inlineStr">
-        <is>
-          <t>Michoel ben Yosef</t>
-        </is>
-      </c>
+      <c r="D1467" t="inlineStr"/>
       <c r="E1467" t="n">
         <v>35</v>
       </c>
@@ -28504,7 +29068,11 @@
           <t>June 3 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D1468" t="inlineStr"/>
+      <c r="D1468" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E1468" t="n">
         <v>35</v>
       </c>
@@ -28523,7 +29091,11 @@
           <t>June 3 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D1469" t="inlineStr"/>
+      <c r="D1469" t="inlineStr">
+        <is>
+          <t>Jerry Kaiser</t>
+        </is>
+      </c>
       <c r="E1469" t="n">
         <v>35</v>
       </c>
@@ -28618,7 +29190,11 @@
           <t>June 4 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D1474" t="inlineStr"/>
+      <c r="D1474" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E1474" t="n">
         <v>35</v>
       </c>
@@ -28637,7 +29213,11 @@
           <t>June 4 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D1475" t="inlineStr"/>
+      <c r="D1475" t="inlineStr">
+        <is>
+          <t>Murray Tuckman</t>
+        </is>
+      </c>
       <c r="E1475" t="n">
         <v>35</v>
       </c>
@@ -28751,7 +29331,11 @@
           <t>June 5 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D1481" t="inlineStr"/>
+      <c r="D1481" t="inlineStr">
+        <is>
+          <t>Happy Birthday</t>
+        </is>
+      </c>
       <c r="E1481" t="n">
         <v>35</v>
       </c>
@@ -28770,7 +29354,11 @@
           <t>June 5 - Line 4 (35)</t>
         </is>
       </c>
-      <c r="D1482" t="inlineStr"/>
+      <c r="D1482" t="inlineStr">
+        <is>
+          <t>Kathryn Safran</t>
+        </is>
+      </c>
       <c r="E1482" t="n">
         <v>35</v>
       </c>
@@ -28903,11 +29491,7 @@
           <t>June 6 - Line 3 (35)</t>
         </is>
       </c>
-      <c r="D1489" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Yahrtzeit of </t>
-        </is>
-      </c>
+      <c r="D1489" t="inlineStr"/>
       <c r="E1489" t="n">
         <v>35</v>
       </c>
@@ -28926,11 +29510,7 @@
           <t>June 6 - Line 2 (35)</t>
         </is>
       </c>
-      <c r="D1490" t="inlineStr">
-        <is>
-          <t>Yeshayahu ben Avrohom Jodorcovsky</t>
-        </is>
-      </c>
+      <c r="D1490" t="inlineStr"/>
       <c r="E1490" t="n">
         <v>35</v>
       </c>
@@ -28949,11 +29529,7 @@
           <t>June 6 - Line 1 (35)</t>
         </is>
       </c>
-      <c r="D1491" t="inlineStr">
-        <is>
-          <t>Yahrtzeit of Charlotte Schwartz</t>
-        </is>
-      </c>
+      <c r="D1491" t="inlineStr"/>
       <c r="E1491" t="n">
         <v>35</v>
       </c>
@@ -28991,11 +29567,7 @@
           <t>June 7 - Line 2 (35)</t>
         </is>
       </c>
-      <c r="D1493" t="inlineStr">
-        <is>
-          <t>Happy Birthday Eden (Sophia)</t>
-        </is>
-      </c>
+      <c r="D1493" t="inlineStr"/>
       <c r="E1493" t="n">
         <v>35</v>
       </c>
@@ -29071,7 +29643,11 @@
           <t>June 8 - Line 1 (35)</t>
         </is>
       </c>
-      <c r="D1497" t="inlineStr"/>
+      <c r="D1497" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E1497" t="n">
         <v>35</v>
       </c>
@@ -29166,11 +29742,7 @@
           <t>June 9 - Line 2 (35)</t>
         </is>
       </c>
-      <c r="D1502" t="inlineStr">
-        <is>
-          <t>Yahtzeit of Meer Friedman</t>
-        </is>
-      </c>
+      <c r="D1502" t="inlineStr"/>
       <c r="E1502" t="n">
         <v>35</v>
       </c>
@@ -29189,11 +29761,7 @@
           <t>June 9 - Line 1 (35)</t>
         </is>
       </c>
-      <c r="D1503" t="inlineStr">
-        <is>
-          <t>Mayer ben Chaim</t>
-        </is>
-      </c>
+      <c r="D1503" t="inlineStr"/>
       <c r="E1503" t="n">
         <v>35</v>
       </c>
@@ -29668,7 +30236,11 @@
           <t>June 15 - Line 5 (25)</t>
         </is>
       </c>
-      <c r="D1528" t="inlineStr"/>
+      <c r="D1528" t="inlineStr">
+        <is>
+          <t>Mendel Leverton</t>
+        </is>
+      </c>
       <c r="E1528" t="n">
         <v>25</v>
       </c>
@@ -29782,11 +30354,7 @@
           <t>June 16 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D1534" t="inlineStr">
-        <is>
-          <t>Yahrtzeit of Bubby Notik</t>
-        </is>
-      </c>
+      <c r="D1534" t="inlineStr"/>
       <c r="E1534" t="n">
         <v>35</v>
       </c>
@@ -29805,11 +30373,7 @@
           <t>June 16 - Line 4 (35)</t>
         </is>
       </c>
-      <c r="D1535" t="inlineStr">
-        <is>
-          <t>Rivka Sheina bas R' Saadya</t>
-        </is>
-      </c>
+      <c r="D1535" t="inlineStr"/>
       <c r="E1535" t="n">
         <v>35</v>
       </c>
@@ -29847,11 +30411,7 @@
           <t>June 16 - Line 2 (35)</t>
         </is>
       </c>
-      <c r="D1537" t="inlineStr">
-        <is>
-          <t>Yahrtzeit of Abe Horovitz</t>
-        </is>
-      </c>
+      <c r="D1537" t="inlineStr"/>
       <c r="E1537" t="n">
         <v>35</v>
       </c>
@@ -29870,11 +30430,7 @@
           <t>June 16 - Line 1 (35)</t>
         </is>
       </c>
-      <c r="D1538" t="inlineStr">
-        <is>
-          <t>Avraham ben Tzvi</t>
-        </is>
-      </c>
+      <c r="D1538" t="inlineStr"/>
       <c r="E1538" t="n">
         <v>35</v>
       </c>
@@ -29893,7 +30449,11 @@
           <t>June 17 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D1539" t="inlineStr"/>
+      <c r="D1539" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E1539" t="n">
         <v>35</v>
       </c>
@@ -29912,7 +30472,11 @@
           <t>June 17 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D1540" t="inlineStr"/>
+      <c r="D1540" t="inlineStr">
+        <is>
+          <t>Donna Rudnick</t>
+        </is>
+      </c>
       <c r="E1540" t="n">
         <v>35</v>
       </c>
@@ -30330,11 +30894,7 @@
           <t>June 20 - Line 1 (35)</t>
         </is>
       </c>
-      <c r="D1562" t="inlineStr">
-        <is>
-          <t>Yahrtzeit of Fiby Amar</t>
-        </is>
-      </c>
+      <c r="D1562" t="inlineStr"/>
       <c r="E1562" t="n">
         <v>35</v>
       </c>
@@ -30904,11 +31464,7 @@
           <t>June 26 - Line 2 (35)</t>
         </is>
       </c>
-      <c r="D1592" t="inlineStr">
-        <is>
-          <t>Happy Birthday</t>
-        </is>
-      </c>
+      <c r="D1592" t="inlineStr"/>
       <c r="E1592" t="n">
         <v>35</v>
       </c>
@@ -30927,11 +31483,7 @@
           <t>June 26 - Line 1 (35)</t>
         </is>
       </c>
-      <c r="D1593" t="inlineStr">
-        <is>
-          <t>Aryeh (Charles) Schiller</t>
-        </is>
-      </c>
+      <c r="D1593" t="inlineStr"/>
       <c r="E1593" t="n">
         <v>35</v>
       </c>
@@ -31007,11 +31559,7 @@
           <t>June 27 - Line 3 (35)</t>
         </is>
       </c>
-      <c r="D1597" t="inlineStr">
-        <is>
-          <t>Happy Birthday Sarah</t>
-        </is>
-      </c>
+      <c r="D1597" t="inlineStr"/>
       <c r="E1597" t="n">
         <v>35</v>
       </c>
@@ -31049,11 +31597,7 @@
           <t>June 27 - Line 1 (35)</t>
         </is>
       </c>
-      <c r="D1599" t="inlineStr">
-        <is>
-          <t>Happy Birthday Ahuva (Amanda) Beker</t>
-        </is>
-      </c>
+      <c r="D1599" t="inlineStr"/>
       <c r="E1599" t="n">
         <v>35</v>
       </c>
@@ -31395,7 +31939,11 @@
           <t>July 2 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D1617" t="inlineStr"/>
+      <c r="D1617" t="inlineStr">
+        <is>
+          <t>Happy Anniversary</t>
+        </is>
+      </c>
       <c r="E1617" t="n">
         <v>35</v>
       </c>
@@ -31414,7 +31962,11 @@
           <t>July 2 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D1618" t="inlineStr"/>
+      <c r="D1618" t="inlineStr">
+        <is>
+          <t>Steve &amp; Gail Tuckman</t>
+        </is>
+      </c>
       <c r="E1618" t="n">
         <v>35</v>
       </c>
@@ -31737,7 +32289,11 @@
           <t>July 5 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D1635" t="inlineStr"/>
+      <c r="D1635" t="inlineStr">
+        <is>
+          <t>Happy Birthday</t>
+        </is>
+      </c>
       <c r="E1635" t="n">
         <v>35</v>
       </c>
@@ -31756,7 +32312,11 @@
           <t>July 5 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D1636" t="inlineStr"/>
+      <c r="D1636" t="inlineStr">
+        <is>
+          <t>Dan Bershad</t>
+        </is>
+      </c>
       <c r="E1636" t="n">
         <v>35</v>
       </c>
@@ -31965,11 +32525,7 @@
           <t>July 7 - Line 2 (35)</t>
         </is>
       </c>
-      <c r="D1647" t="inlineStr">
-        <is>
-          <t>Yahrtzeit of Sonny Steinman</t>
-        </is>
-      </c>
+      <c r="D1647" t="inlineStr"/>
       <c r="E1647" t="n">
         <v>35</v>
       </c>
@@ -31988,11 +32544,7 @@
           <t>July 7 - Line 1 (35)</t>
         </is>
       </c>
-      <c r="D1648" t="inlineStr">
-        <is>
-          <t>Yitzchak ben Dovid</t>
-        </is>
-      </c>
+      <c r="D1648" t="inlineStr"/>
       <c r="E1648" t="n">
         <v>35</v>
       </c>
@@ -32391,7 +32943,11 @@
           <t xml:space="preserve">July 11 - Line 4 (35) </t>
         </is>
       </c>
-      <c r="D1669" t="inlineStr"/>
+      <c r="D1669" t="inlineStr">
+        <is>
+          <t>Happy Anniversary</t>
+        </is>
+      </c>
       <c r="E1669" t="n">
         <v>35</v>
       </c>
@@ -32410,7 +32966,11 @@
           <t>July 11 - Line 3 (35)</t>
         </is>
       </c>
-      <c r="D1670" t="inlineStr"/>
+      <c r="D1670" t="inlineStr">
+        <is>
+          <t>Miles &amp; Sheryl Martin</t>
+        </is>
+      </c>
       <c r="E1670" t="n">
         <v>35</v>
       </c>
@@ -32467,7 +33027,11 @@
           <t>July 12 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D1673" t="inlineStr"/>
+      <c r="D1673" t="inlineStr">
+        <is>
+          <t>Happy Birthday</t>
+        </is>
+      </c>
       <c r="E1673" t="n">
         <v>35</v>
       </c>
@@ -32486,7 +33050,11 @@
           <t>July 12 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D1674" t="inlineStr"/>
+      <c r="D1674" t="inlineStr">
+        <is>
+          <t>Tal Kalif</t>
+        </is>
+      </c>
       <c r="E1674" t="n">
         <v>35</v>
       </c>
@@ -33626,7 +34194,11 @@
           <t>July 23 - Line 4 (35)</t>
         </is>
       </c>
-      <c r="D1734" t="inlineStr"/>
+      <c r="D1734" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E1734" t="n">
         <v>35</v>
       </c>
@@ -33645,7 +34217,11 @@
           <t>July 23 - Line 3 (35)</t>
         </is>
       </c>
-      <c r="D1735" t="inlineStr"/>
+      <c r="D1735" t="inlineStr">
+        <is>
+          <t>Beatrice Schwartz</t>
+        </is>
+      </c>
       <c r="E1735" t="n">
         <v>35</v>
       </c>
@@ -33930,7 +34506,11 @@
           <t>July 26 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D1750" t="inlineStr"/>
+      <c r="D1750" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E1750" t="n">
         <v>35</v>
       </c>
@@ -33949,7 +34529,11 @@
           <t>July 26 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D1751" t="inlineStr"/>
+      <c r="D1751" t="inlineStr">
+        <is>
+          <t>Bella Finkelstein</t>
+        </is>
+      </c>
       <c r="E1751" t="n">
         <v>35</v>
       </c>
@@ -34120,7 +34704,11 @@
           <t>July 28 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D1760" t="inlineStr"/>
+      <c r="D1760" t="inlineStr">
+        <is>
+          <t>Happy Birthday</t>
+        </is>
+      </c>
       <c r="E1760" t="n">
         <v>35</v>
       </c>
@@ -34139,7 +34727,11 @@
           <t>July 28 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D1761" t="inlineStr"/>
+      <c r="D1761" t="inlineStr">
+        <is>
+          <t>Natalie Abayev</t>
+        </is>
+      </c>
       <c r="E1761" t="n">
         <v>35</v>
       </c>
@@ -34215,11 +34807,7 @@
           <t>July 28 - Line 1 (35)</t>
         </is>
       </c>
-      <c r="D1765" t="inlineStr">
-        <is>
-          <t>Yahrtzeit of Jacques Bendahan</t>
-        </is>
-      </c>
+      <c r="D1765" t="inlineStr"/>
       <c r="E1765" t="n">
         <v>35</v>
       </c>
@@ -34238,7 +34826,11 @@
           <t>July 29 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D1766" t="inlineStr"/>
+      <c r="D1766" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E1766" t="n">
         <v>35</v>
       </c>
@@ -34257,7 +34849,11 @@
           <t>July 29 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D1767" t="inlineStr"/>
+      <c r="D1767" t="inlineStr">
+        <is>
+          <t>Lillian Goldfarb</t>
+        </is>
+      </c>
       <c r="E1767" t="n">
         <v>35</v>
       </c>
@@ -34808,7 +35404,11 @@
           <t>August 3 - Line 4 (25)</t>
         </is>
       </c>
-      <c r="D1796" t="inlineStr"/>
+      <c r="D1796" t="inlineStr">
+        <is>
+          <t>Happy Birthday</t>
+        </is>
+      </c>
       <c r="E1796" t="n">
         <v>25</v>
       </c>
@@ -34827,7 +35427,11 @@
           <t>August 3 - Line 3 (35)</t>
         </is>
       </c>
-      <c r="D1797" t="inlineStr"/>
+      <c r="D1797" t="inlineStr">
+        <is>
+          <t>Ari Leverton</t>
+        </is>
+      </c>
       <c r="E1797" t="n">
         <v>35</v>
       </c>
@@ -34884,7 +35488,11 @@
           <t>August 4 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D1800" t="inlineStr"/>
+      <c r="D1800" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E1800" t="n">
         <v>35</v>
       </c>
@@ -34903,7 +35511,11 @@
           <t>August 4 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D1801" t="inlineStr"/>
+      <c r="D1801" t="inlineStr">
+        <is>
+          <t>Fred M. Cohen</t>
+        </is>
+      </c>
       <c r="E1801" t="n">
         <v>35</v>
       </c>
@@ -35093,7 +35705,11 @@
           <t>August 6 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D1811" t="inlineStr"/>
+      <c r="D1811" t="inlineStr">
+        <is>
+          <t>Happy Birthday</t>
+        </is>
+      </c>
       <c r="E1811" t="n">
         <v>35</v>
       </c>
@@ -35112,7 +35728,11 @@
           <t>August 6 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D1812" t="inlineStr"/>
+      <c r="D1812" t="inlineStr">
+        <is>
+          <t>Helene Wishnev</t>
+        </is>
+      </c>
       <c r="E1812" t="n">
         <v>35</v>
       </c>
@@ -35169,11 +35789,7 @@
           <t>August 6 - Line 2 (35)</t>
         </is>
       </c>
-      <c r="D1815" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Yahrtzeit of </t>
-        </is>
-      </c>
+      <c r="D1815" t="inlineStr"/>
       <c r="E1815" t="n">
         <v>35</v>
       </c>
@@ -35192,11 +35808,7 @@
           <t>August 6 - Line 1 (35)</t>
         </is>
       </c>
-      <c r="D1816" t="inlineStr">
-        <is>
-          <t>Aimee Madeline Richmond</t>
-        </is>
-      </c>
+      <c r="D1816" t="inlineStr"/>
       <c r="E1816" t="n">
         <v>35</v>
       </c>
@@ -35614,7 +36226,11 @@
           <t>August 11 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D1838" t="inlineStr"/>
+      <c r="D1838" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E1838" t="n">
         <v>35</v>
       </c>
@@ -35633,7 +36249,11 @@
           <t>August 11 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D1839" t="inlineStr"/>
+      <c r="D1839" t="inlineStr">
+        <is>
+          <t>Robert Wishnev</t>
+        </is>
+      </c>
       <c r="E1839" t="n">
         <v>35</v>
       </c>
@@ -35823,7 +36443,11 @@
           <t>August 13 - Line 6 (20)</t>
         </is>
       </c>
-      <c r="D1849" t="inlineStr"/>
+      <c r="D1849" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E1849" t="n">
         <v>20</v>
       </c>
@@ -35842,7 +36466,11 @@
           <t>August 13 - Line 5 (20)</t>
         </is>
       </c>
-      <c r="D1850" t="inlineStr"/>
+      <c r="D1850" t="inlineStr">
+        <is>
+          <t>Marsha Golbert Pannone</t>
+        </is>
+      </c>
       <c r="E1850" t="n">
         <v>20</v>
       </c>
@@ -36564,7 +37192,11 @@
           <t>August 20 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D1888" t="inlineStr"/>
+      <c r="D1888" t="inlineStr">
+        <is>
+          <t>Happy Birthday</t>
+        </is>
+      </c>
       <c r="E1888" t="n">
         <v>35</v>
       </c>
@@ -36583,7 +37215,11 @@
           <t>August 20 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D1889" t="inlineStr"/>
+      <c r="D1889" t="inlineStr">
+        <is>
+          <t>Jaya Abayev</t>
+        </is>
+      </c>
       <c r="E1889" t="n">
         <v>35</v>
       </c>
@@ -36678,7 +37314,11 @@
           <t>August 21 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D1894" t="inlineStr"/>
+      <c r="D1894" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E1894" t="n">
         <v>35</v>
       </c>
@@ -36697,7 +37337,11 @@
           <t>August 21 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D1895" t="inlineStr"/>
+      <c r="D1895" t="inlineStr">
+        <is>
+          <t>Bernard Saltin</t>
+        </is>
+      </c>
       <c r="E1895" t="n">
         <v>35</v>
       </c>
@@ -37210,7 +37854,11 @@
           <t>August 26 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D1922" t="inlineStr"/>
+      <c r="D1922" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E1922" t="n">
         <v>35</v>
       </c>
@@ -37229,7 +37877,11 @@
           <t>August 26 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D1923" t="inlineStr"/>
+      <c r="D1923" t="inlineStr">
+        <is>
+          <t>Shirlee Goldfarb</t>
+        </is>
+      </c>
       <c r="E1923" t="n">
         <v>35</v>
       </c>
@@ -37666,7 +38318,11 @@
           <t>August 30 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D1946" t="inlineStr"/>
+      <c r="D1946" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E1946" t="n">
         <v>35</v>
       </c>
@@ -37685,7 +38341,11 @@
           <t>August 30 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D1947" t="inlineStr"/>
+      <c r="D1947" t="inlineStr">
+        <is>
+          <t>Carl H. Grill</t>
+        </is>
+      </c>
       <c r="E1947" t="n">
         <v>35</v>
       </c>
@@ -38654,7 +39314,11 @@
           <t>September 9 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D1998" t="inlineStr"/>
+      <c r="D1998" t="inlineStr">
+        <is>
+          <t>Happy Birthday</t>
+        </is>
+      </c>
       <c r="E1998" t="n">
         <v>35</v>
       </c>
@@ -38673,7 +39337,11 @@
           <t>September 9 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D1999" t="inlineStr"/>
+      <c r="D1999" t="inlineStr">
+        <is>
+          <t>Ella Kalif</t>
+        </is>
+      </c>
       <c r="E1999" t="n">
         <v>35</v>
       </c>
@@ -38768,7 +39436,11 @@
           <t>September 10 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D2004" t="inlineStr"/>
+      <c r="D2004" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E2004" t="n">
         <v>35</v>
       </c>
@@ -38787,7 +39459,11 @@
           <t>September 10 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D2005" t="inlineStr"/>
+      <c r="D2005" t="inlineStr">
+        <is>
+          <t>Max Herman</t>
+        </is>
+      </c>
       <c r="E2005" t="n">
         <v>35</v>
       </c>
@@ -38806,7 +39482,11 @@
           <t>September 10 - Line 4 (35)</t>
         </is>
       </c>
-      <c r="D2006" t="inlineStr"/>
+      <c r="D2006" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E2006" t="n">
         <v>35</v>
       </c>
@@ -38825,7 +39505,11 @@
           <t>September 10 - Line 3 (35)</t>
         </is>
       </c>
-      <c r="D2007" t="inlineStr"/>
+      <c r="D2007" t="inlineStr">
+        <is>
+          <t>Arthur Finkelstein</t>
+        </is>
+      </c>
       <c r="E2007" t="n">
         <v>35</v>
       </c>
@@ -38844,7 +39528,11 @@
           <t>September 10 - Line 2 (35)</t>
         </is>
       </c>
-      <c r="D2008" t="inlineStr"/>
+      <c r="D2008" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E2008" t="n">
         <v>35</v>
       </c>
@@ -38863,7 +39551,11 @@
           <t>September 10 - Line 1 (35)</t>
         </is>
       </c>
-      <c r="D2009" t="inlineStr"/>
+      <c r="D2009" t="inlineStr">
+        <is>
+          <t>Arthur Finkelstein</t>
+        </is>
+      </c>
       <c r="E2009" t="n">
         <v>35</v>
       </c>
@@ -39300,7 +39992,11 @@
           <t>September 15 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D2032" t="inlineStr"/>
+      <c r="D2032" t="inlineStr">
+        <is>
+          <t>Happy Birthday</t>
+        </is>
+      </c>
       <c r="E2032" t="n">
         <v>35</v>
       </c>
@@ -39319,7 +40015,11 @@
           <t>September 15 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D2033" t="inlineStr"/>
+      <c r="D2033" t="inlineStr">
+        <is>
+          <t>Beatrice Gilhart</t>
+        </is>
+      </c>
       <c r="E2033" t="n">
         <v>35</v>
       </c>
@@ -39338,7 +40038,11 @@
           <t>September 15 - Line 4 (35)</t>
         </is>
       </c>
-      <c r="D2034" t="inlineStr"/>
+      <c r="D2034" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E2034" t="n">
         <v>35</v>
       </c>
@@ -39357,7 +40061,11 @@
           <t>September 15 - Line 3 (35)</t>
         </is>
       </c>
-      <c r="D2035" t="inlineStr"/>
+      <c r="D2035" t="inlineStr">
+        <is>
+          <t>Beatrice Gilhart</t>
+        </is>
+      </c>
       <c r="E2035" t="n">
         <v>35</v>
       </c>
@@ -39794,7 +40502,11 @@
           <t>September 19 - Line 4 (35)</t>
         </is>
       </c>
-      <c r="D2058" t="inlineStr"/>
+      <c r="D2058" t="inlineStr">
+        <is>
+          <t>Happy Birthday</t>
+        </is>
+      </c>
       <c r="E2058" t="n">
         <v>35</v>
       </c>
@@ -39813,7 +40525,11 @@
           <t>September 19 - Line 3 (35)</t>
         </is>
       </c>
-      <c r="D2059" t="inlineStr"/>
+      <c r="D2059" t="inlineStr">
+        <is>
+          <t>Ella Kalif</t>
+        </is>
+      </c>
       <c r="E2059" t="n">
         <v>35</v>
       </c>
@@ -40383,11 +41099,7 @@
           <t>September 24 - Line 1 (35)</t>
         </is>
       </c>
-      <c r="D2089" t="inlineStr">
-        <is>
-          <t>Yahrtzeit of Libby Echenberg</t>
-        </is>
-      </c>
+      <c r="D2089" t="inlineStr"/>
       <c r="E2089" t="n">
         <v>35</v>
       </c>
@@ -40767,11 +41479,7 @@
           <t>September 28 - Line 2 (35)</t>
         </is>
       </c>
-      <c r="D2109" t="inlineStr">
-        <is>
-          <t>Yahrtzeit of Felicia Aaron</t>
-        </is>
-      </c>
+      <c r="D2109" t="inlineStr"/>
       <c r="E2109" t="n">
         <v>35</v>
       </c>
@@ -40790,11 +41498,7 @@
           <t>September 28 - Line 1 (35)</t>
         </is>
       </c>
-      <c r="D2110" t="inlineStr">
-        <is>
-          <t>Tzipora Bas Shimon Leib</t>
-        </is>
-      </c>
+      <c r="D2110" t="inlineStr"/>
       <c r="E2110" t="n">
         <v>35</v>
       </c>
@@ -40813,7 +41517,11 @@
           <t>September 29 - Line 6 (35)</t>
         </is>
       </c>
-      <c r="D2111" t="inlineStr"/>
+      <c r="D2111" t="inlineStr">
+        <is>
+          <t>Yahrtzeit</t>
+        </is>
+      </c>
       <c r="E2111" t="n">
         <v>35</v>
       </c>
@@ -40832,7 +41540,11 @@
           <t>September 29 - Line 5 (35)</t>
         </is>
       </c>
-      <c r="D2112" t="inlineStr"/>
+      <c r="D2112" t="inlineStr">
+        <is>
+          <t>Larry Barnett</t>
+        </is>
+      </c>
       <c r="E2112" t="n">
         <v>35</v>
       </c>

</xml_diff>